<commit_message>
finished script to run all parsers and evaluate on ctb
</commit_message>
<xml_diff>
--- a/jiebaPOS.xlsx
+++ b/jiebaPOS.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Smith-Box/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Smith-Box/Documents/chinese_orca/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="zho" sheetId="1" r:id="rId1"/>
@@ -433,9 +433,6 @@
     <t>Take the first letter of the English conjunction conjunction.</t>
   </si>
   <si>
-    <t>Vice morpheme</t>
-  </si>
-  <si>
     <t>Adverbial morpheme. Adverb code d, morpheme code g front set to D.</t>
   </si>
   <si>
@@ -544,9 +541,6 @@
     <t>Take the first letter of the prepositional English prepositional.</t>
   </si>
   <si>
-    <t>quantifier</t>
-  </si>
-  <si>
     <t>Take the first letter of the English quantity.</t>
   </si>
   <si>
@@ -590,9 +584,6 @@
   </si>
   <si>
     <t>Take the first letter of the English verb verb.</t>
-  </si>
-  <si>
-    <t>Deputy verb</t>
   </si>
   <si>
     <t>Verbs that are directly adverbial. Verb and adverb code together.</t>
@@ -640,6 +631,15 @@
       </rPr>
       <t>(Non-Peking University standards, as defined in the CSW participle)</t>
     </r>
+  </si>
+  <si>
+    <t>quantifier/measure words</t>
+  </si>
+  <si>
+    <t>Auxiliary verb</t>
+  </si>
+  <si>
+    <t>averbial morpheme</t>
   </si>
 </sst>
 </file>
@@ -978,7 +978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1430,7 +1430,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1508,10 +1510,10 @@
         <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1519,10 +1521,10 @@
         <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1530,10 +1532,10 @@
         <v>24</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1541,10 +1543,10 @@
         <v>27</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1552,10 +1554,10 @@
         <v>30</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1563,10 +1565,10 @@
         <v>33</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1574,10 +1576,10 @@
         <v>36</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1585,10 +1587,10 @@
         <v>39</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1596,7 +1598,7 @@
         <v>42</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C15" s="3"/>
     </row>
@@ -1605,10 +1607,10 @@
         <v>44</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1616,10 +1618,10 @@
         <v>47</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1627,10 +1629,10 @@
         <v>50</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1638,10 +1640,10 @@
         <v>53</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1649,10 +1651,10 @@
         <v>56</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>155</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1660,10 +1662,10 @@
         <v>59</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1671,10 +1673,10 @@
         <v>62</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>159</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1682,10 +1684,10 @@
         <v>65</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1693,10 +1695,10 @@
         <v>68</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>163</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1704,10 +1706,10 @@
         <v>71</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>165</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1715,10 +1717,10 @@
         <v>74</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1726,10 +1728,10 @@
         <v>77</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1737,10 +1739,10 @@
         <v>80</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1748,10 +1750,10 @@
         <v>83</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1759,10 +1761,10 @@
         <v>86</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1770,10 +1772,10 @@
         <v>89</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1781,10 +1783,10 @@
         <v>92</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1792,10 +1794,10 @@
         <v>95</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1803,10 +1805,10 @@
         <v>98</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1814,10 +1816,10 @@
         <v>101</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1825,7 +1827,7 @@
         <v>104</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C36" s="3"/>
     </row>
@@ -1834,10 +1836,10 @@
         <v>106</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1845,10 +1847,10 @@
         <v>109</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1856,10 +1858,10 @@
         <v>112</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -1867,10 +1869,10 @@
         <v>115</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>